<commit_message>
doc classifier intial commit
</commit_message>
<xml_diff>
--- a/reports/XRP_DMCR_Reporting dataset_v02.xlsx
+++ b/reports/XRP_DMCR_Reporting dataset_v02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\QUALCO PROJECTS\Computational Solutions R&amp;D\Collaborations &amp; Third Party Contributions\Demokritos\MSc 2022-2023\Data dictionaries and reports\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avitsas\Documents\thesis-backup\thesis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F51381C-4AEB-41A6-B707-394EA5812354}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E126B1C7-4D57-4F36-9B10-B257ABB5C4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{3D93E94A-893C-4924-AB58-450630FF5BB4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{3D93E94A-893C-4924-AB58-450630FF5BB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment predictions 1" sheetId="2" r:id="rId1"/>
@@ -2081,7 +2081,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2406,9 +2406,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -2647,9 +2644,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -3103,9 +3097,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -3556,9 +3547,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -3749,9 +3737,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -3759,8 +3744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160D6B06-C3BC-4CD2-BE33-1547D2F7DE00}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4509,9 +4494,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -4519,7 +4501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295564AD-6354-4181-A6A5-528C8B05A469}">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5275,9 +5257,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -6056,9 +6035,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -6827,8 +6803,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;16&amp;K0000FFRESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
measure patterns initial commit
</commit_message>
<xml_diff>
--- a/reports/XRP_DMCR_Reporting dataset_v02.xlsx
+++ b/reports/XRP_DMCR_Reporting dataset_v02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avitsas\Documents\thesis-backup\thesis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E126B1C7-4D57-4F36-9B10-B257ABB5C4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45A880E-0B94-4318-8BFE-8F2BD773388F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{3D93E94A-893C-4924-AB58-450630FF5BB4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{3D93E94A-893C-4924-AB58-450630FF5BB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment predictions 1" sheetId="2" r:id="rId1"/>
@@ -2080,13 +2080,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA722898-DFA4-4F83-B933-650728FDFACA}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="60.21875" customWidth="1"/>
+    <col min="4" max="4" width="82.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2414,7 +2415,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2652,18 +2653,18 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="42.21875" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" customWidth="1"/>
     <col min="8" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3104,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC1C392-DE55-4D73-A17F-56FDF49E25CE}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3117,7 +3118,7 @@
     <col min="8" max="8" width="30.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3745,7 +3746,7 @@
   <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4501,8 +4502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295564AD-6354-4181-A6A5-528C8B05A469}">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5264,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4DF90B-81B4-4B1B-8E2E-EB4119F6AC63}">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6042,8 +6043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DD82C4-2B2E-4DA0-A6DE-399029A942DC}">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>